<commit_message>
modificacion de datasource y test run
</commit_message>
<xml_diff>
--- a/SuraClaims/Pago_Siniestros_Motor.xlsx
+++ b/SuraClaims/Pago_Siniestros_Motor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Sura - Claims\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E176A53-27D6-4837-9040-2F51EF318F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F72C3F4-A40B-412E-B42F-B0FEC3A7A876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Usuario</t>
   </si>
@@ -69,12 +69,6 @@
     <t>0420172006736</t>
   </si>
   <si>
-    <t>1120170200879</t>
-  </si>
-  <si>
-    <t>1220170301317</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -82,12 +76,6 @@
   </si>
   <si>
     <t>Parcial</t>
-  </si>
-  <si>
-    <t>Incendio</t>
-  </si>
-  <si>
-    <t>Lesion y Medicinas</t>
   </si>
 </sst>
 </file>
@@ -439,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -490,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -513,58 +501,12 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -572,10 +514,8 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{2A9678FE-A5C3-4D99-A66A-79151093C407}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{1D6CA312-C3C5-43DF-94EF-DD26B1362890}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{8B06CF65-A7D0-4989-8376-D562CC5E453F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglo de pago de siniestros
</commit_message>
<xml_diff>
--- a/SuraClaims/Pago_Siniestros_Motor.xlsx
+++ b/SuraClaims/Pago_Siniestros_Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73551A64-8D9A-478F-8B94-576BED07E89A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4A062-4B5E-469B-A034-CDB6F1F7E3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Usuario</t>
   </si>
@@ -51,12 +51,6 @@
     <t>0420172007039</t>
   </si>
   <si>
-    <t>i-preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
-    <t>https://i-preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
-  </si>
-  <si>
     <t>MetodoPagoSiniestro</t>
   </si>
   <si>
@@ -78,13 +72,13 @@
     <t>Parcial</t>
   </si>
   <si>
-    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
-  </si>
-  <si>
-    <t>0420194406369</t>
+    <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -436,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,21 +458,21 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -487,21 +481,21 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -510,28 +504,34 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{2A9678FE-A5C3-4D99-A66A-79151093C407}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CC1A8AFD-B359-4838-A3AF-5A3E300A1143}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0BFC63D6-82FE-45E6-923E-085F2A6F2FDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>